<commit_message>
Added multiple room features w guardEq()
status (not implemented)
help (now returns description of roomActions)
sell <amount>
buy <upgrade_name> <amount>
pickup <amount>
hint (not implemented)
</commit_message>
<xml_diff>
--- a/Gantt-projektplanlægger.xlsx
+++ b/Gantt-projektplanlægger.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26731"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="6" documentId="8_{69CB8AA2-1BCC-4B30-A743-A985B93270C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BD5A46FD-4A69-4E68-9A93-3CA4490BEB95}"/>
+  <xr:revisionPtr revIDLastSave="26" documentId="8_{69CB8AA2-1BCC-4B30-A743-A985B93270C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E32F148A-E231-4F5A-898C-19B90D84A516}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -642,6 +642,18 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="2" applyFont="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="9">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="9" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="10">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="10" applyBorder="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -651,9 +663,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="10" applyBorder="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="10" applyBorder="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -668,15 +677,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="9">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="9" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="10">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="19">
@@ -854,10 +854,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1094,7 +1090,7 @@
   <dimension ref="B1:BP30"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="55" zoomScaleNormal="80" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.25" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -1134,69 +1130,69 @@
         <v>1</v>
       </c>
       <c r="K2" s="13"/>
-      <c r="L2" s="31" t="s">
+      <c r="L2" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="M2" s="32"/>
-      <c r="N2" s="32"/>
-      <c r="O2" s="32"/>
-      <c r="P2" s="33"/>
+      <c r="M2" s="35"/>
+      <c r="N2" s="35"/>
+      <c r="O2" s="35"/>
+      <c r="P2" s="36"/>
       <c r="Q2" s="14"/>
-      <c r="R2" s="31" t="s">
+      <c r="R2" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="S2" s="34"/>
-      <c r="T2" s="34"/>
-      <c r="U2" s="34"/>
-      <c r="V2" s="33"/>
+      <c r="S2" s="37"/>
+      <c r="T2" s="37"/>
+      <c r="U2" s="37"/>
+      <c r="V2" s="36"/>
       <c r="W2" s="15"/>
-      <c r="X2" s="27" t="s">
+      <c r="X2" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="Y2" s="28"/>
-      <c r="Z2" s="35"/>
+      <c r="Y2" s="32"/>
+      <c r="Z2" s="38"/>
       <c r="AA2" s="16"/>
-      <c r="AB2" s="27" t="s">
+      <c r="AB2" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="AC2" s="28"/>
-      <c r="AD2" s="28"/>
-      <c r="AE2" s="28"/>
-      <c r="AF2" s="28"/>
-      <c r="AG2" s="28"/>
+      <c r="AC2" s="32"/>
+      <c r="AD2" s="32"/>
+      <c r="AE2" s="32"/>
+      <c r="AF2" s="32"/>
+      <c r="AG2" s="32"/>
       <c r="AH2" s="17"/>
-      <c r="AI2" s="27" t="s">
+      <c r="AI2" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="AJ2" s="28"/>
-      <c r="AK2" s="28"/>
-      <c r="AL2" s="28"/>
-      <c r="AM2" s="28"/>
-      <c r="AN2" s="28"/>
-      <c r="AO2" s="28"/>
+      <c r="AJ2" s="32"/>
+      <c r="AK2" s="32"/>
+      <c r="AL2" s="32"/>
+      <c r="AM2" s="32"/>
+      <c r="AN2" s="32"/>
+      <c r="AO2" s="32"/>
       <c r="AP2" s="20"/>
       <c r="AQ2" s="20"/>
     </row>
     <row r="3" spans="2:68" s="9" customFormat="1" ht="40" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="36" t="s">
+      <c r="B3" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="36" t="s">
+      <c r="C3" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="D3" s="38" t="s">
+      <c r="D3" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="38" t="s">
+      <c r="E3" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="38" t="s">
+      <c r="F3" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="G3" s="38" t="s">
+      <c r="G3" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="H3" s="29" t="s">
+      <c r="H3" s="33" t="s">
         <v>19</v>
       </c>
       <c r="I3" s="18" t="s">
@@ -1223,8 +1219,8 @@
       <c r="AB3" s="8"/>
     </row>
     <row r="4" spans="2:68" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="37"/>
-      <c r="C4" s="37"/>
+      <c r="B4" s="28"/>
+      <c r="C4" s="28"/>
       <c r="D4" s="30"/>
       <c r="E4" s="30"/>
       <c r="F4" s="30"/>
@@ -1481,10 +1477,14 @@
       <c r="E10" s="22">
         <v>2</v>
       </c>
-      <c r="F10" s="22"/>
-      <c r="G10" s="22"/>
+      <c r="F10" s="22">
+        <v>41</v>
+      </c>
+      <c r="G10" s="22">
+        <v>1</v>
+      </c>
       <c r="H10" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="2:68" ht="51" x14ac:dyDescent="0.4">
@@ -1500,10 +1500,14 @@
       <c r="E11" s="22">
         <v>2</v>
       </c>
-      <c r="F11" s="22"/>
-      <c r="G11" s="22"/>
+      <c r="F11" s="22">
+        <v>41</v>
+      </c>
+      <c r="G11" s="22">
+        <v>1</v>
+      </c>
       <c r="H11" s="23">
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="12" spans="2:68" ht="51" x14ac:dyDescent="0.4">
@@ -1519,10 +1523,14 @@
       <c r="E12" s="22">
         <v>2</v>
       </c>
-      <c r="F12" s="22"/>
-      <c r="G12" s="22"/>
+      <c r="F12" s="22">
+        <v>41</v>
+      </c>
+      <c r="G12" s="22">
+        <v>2</v>
+      </c>
       <c r="H12" s="23">
-        <v>0</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="13" spans="2:68" ht="68" x14ac:dyDescent="0.4">
@@ -1538,10 +1546,14 @@
       <c r="E13" s="22">
         <v>4</v>
       </c>
-      <c r="F13" s="22"/>
-      <c r="G13" s="22"/>
+      <c r="F13" s="22">
+        <v>41</v>
+      </c>
+      <c r="G13" s="22">
+        <v>2</v>
+      </c>
       <c r="H13" s="23">
-        <v>0</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="14" spans="2:68" ht="30" customHeight="1" x14ac:dyDescent="0.4">
@@ -1779,18 +1791,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="AI2:AO2"/>
+    <mergeCell ref="H3:H4"/>
+    <mergeCell ref="L2:P2"/>
+    <mergeCell ref="R2:V2"/>
+    <mergeCell ref="X2:Z2"/>
+    <mergeCell ref="AB2:AG2"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="D3:D4"/>
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="F3:F4"/>
     <mergeCell ref="G3:G4"/>
     <mergeCell ref="C3:C4"/>
-    <mergeCell ref="AI2:AO2"/>
-    <mergeCell ref="H3:H4"/>
-    <mergeCell ref="L2:P2"/>
-    <mergeCell ref="R2:V2"/>
-    <mergeCell ref="X2:Z2"/>
-    <mergeCell ref="AB2:AG2"/>
   </mergeCells>
   <conditionalFormatting sqref="B31:BP31">
     <cfRule type="expression" dxfId="9" priority="2">

</xml_diff>